<commit_message>
Rajout de la classe main dans les schémas
</commit_message>
<xml_diff>
--- a/TP6/Q1.2.3.4.xlsx
+++ b/TP6/Q1.2.3.4.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>Calculator</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>Q1.</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>Rmq: On ne peut tester Main car on ne peut l'instancier</t>
   </si>
 </sst>
 </file>
@@ -107,7 +113,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -139,18 +145,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -176,22 +194,22 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>285750</xdr:colOff>
+          <xdr:colOff>276225</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>828675</xdr:colOff>
+          <xdr:colOff>819150</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>85725</xdr:rowOff>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1027" name="Object 3" hidden="1">
+            <xdr:cNvPr id="1029" name="Object 5" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1027"/>
+                  <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -241,22 +259,22 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
+          <xdr:colOff>57150</xdr:colOff>
           <xdr:row>34</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>762000</xdr:colOff>
-          <xdr:row>50</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:colOff>790575</xdr:colOff>
+          <xdr:row>57</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1028" name="Object 4" hidden="1">
+            <xdr:cNvPr id="1030" name="Object 6" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1028"/>
+                  <a14:compatExt spid="_x0000_s1030"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -305,8 +323,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="B25:H32" totalsRowShown="0">
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="B25:I33" totalsRowShown="0">
+  <tableColumns count="8">
     <tableColumn id="1" name="Calculator"/>
     <tableColumn id="2" name="CalculatorImpl"/>
     <tableColumn id="3" name="MyList"/>
@@ -314,14 +332,15 @@
     <tableColumn id="5" name="Elem"/>
     <tableColumn id="6" name="SuiteChainee"/>
     <tableColumn id="7" name="SuiteChaineeImpl"/>
+    <tableColumn id="8" name="Main"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A39:B42" totalsRowShown="0">
-  <autoFilter ref="A39:B42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A39:B43" totalsRowShown="0">
+  <autoFilter ref="A39:B43"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Niveau de test"/>
     <tableColumn id="2" name="Classe(s)"/>
@@ -620,10 +639,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,7 +670,7 @@
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>12</v>
       </c>
@@ -662,8 +681,9 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
-    </row>
-    <row r="25" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" t="s">
         <v>0</v>
@@ -686,8 +706,11 @@
       <c r="H25" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -697,16 +720,22 @@
       <c r="H26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
@@ -716,16 +745,22 @@
       <c r="H28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>4</v>
       </c>
@@ -735,18 +770,32 @@
       <c r="H30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -796,14 +845,39 @@
         <v>11</v>
       </c>
     </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>4</v>
+      </c>
+      <c r="B43" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A24:H24"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="D34:G34"/>
     <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A24:I24"/>
   </mergeCells>
-  <conditionalFormatting sqref="B26:H32">
+  <conditionalFormatting sqref="B26:H33">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26:I33">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -816,58 +890,58 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="83" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="76" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
   <oleObjects>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Visio.Drawing.15" shapeId="1027" r:id="rId4">
+        <oleObject progId="Visio.Drawing.15" shapeId="1029" r:id="rId4">
           <objectPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>285750</xdr:colOff>
+                <xdr:colOff>276225</xdr:colOff>
                 <xdr:row>1</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:rowOff>38100</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>7</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
+                <xdr:colOff>819150</xdr:colOff>
                 <xdr:row>22</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Visio.Drawing.15" shapeId="1027" r:id="rId4"/>
+        <oleObject progId="Visio.Drawing.15" shapeId="1029" r:id="rId4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Visio.Drawing.15" shapeId="1028" r:id="rId6">
+        <oleObject progId="Visio.Drawing.15" shapeId="1030" r:id="rId6">
           <objectPr defaultSize="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
+                <xdr:colOff>57150</xdr:colOff>
                 <xdr:row>34</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:rowOff>38100</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>762000</xdr:colOff>
-                <xdr:row>50</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:colOff>790575</xdr:colOff>
+                <xdr:row>57</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Visio.Drawing.15" shapeId="1028" r:id="rId6"/>
+        <oleObject progId="Visio.Drawing.15" shapeId="1030" r:id="rId6"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>

</xml_diff>